<commit_message>
new excel code added in a class
</commit_message>
<xml_diff>
--- a/Test Data/ExcelTask.xlsx
+++ b/Test Data/ExcelTask.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\120190\Documents\Personal\SW\Sample Automation\SampleRepoDev\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A42033-5241-48ED-B5BD-80B17DE5BAB8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AB6F33-4747-4DD0-BD3F-C883C6C8DA66}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4875" yWindow="1755" windowWidth="13455" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>egg</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>maavu, garbage bag</t>
+  </si>
+  <si>
+    <t>testxxxxx</t>
   </si>
 </sst>
 </file>
@@ -387,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,8 +494,8 @@
       <c r="C5">
         <v>50</v>
       </c>
-      <c r="D5">
-        <v>5</v>
+      <c r="D5" t="s">
+        <v>15</v>
       </c>
       <c r="E5">
         <v>173</v>
@@ -606,19 +609,24 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1</v>
+      <c r="A19" t="s">
+        <v>15</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>1</v>
+      <c r="A20" t="s">
+        <v>15</v>
       </c>
       <c r="B20" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Excel Read write completed
</commit_message>
<xml_diff>
--- a/Test Data/ExcelTask.xlsx
+++ b/Test Data/ExcelTask.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\120190\Documents\Personal\SW\Sample Automation\SampleRepoDev\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AB6F33-4747-4DD0-BD3F-C883C6C8DA66}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864C8317-F205-40B7-9002-D5C9E0ED09B6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4875" yWindow="1755" windowWidth="13455" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19080" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -108,8 +108,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,15 +391,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -629,6 +630,16 @@
         <v>15</v>
       </c>
     </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>43896</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1111.223</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>